<commit_message>
convert newline in cell into <br/>; support table aligin option `-a [l,c,r]`
</commit_message>
<xml_diff>
--- a/src/test/test1.1.xlsx
+++ b/src/test/test1.1.xlsx
@@ -1,20 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="153222"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28315"/>
+  <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev\code_git_me\exceltk\src\Exceltk\bin\Debug\test\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/feilong/Desktop/dev/exceltk/src/test/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="10890"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="21600" windowHeight="10900"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="7" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -45,9 +53,6 @@
     <t>车超杰</t>
   </si>
   <si>
-    <t>陈安怡</t>
-  </si>
-  <si>
     <t>陆晓鹏</t>
   </si>
   <si>
@@ -145,6 +150,11 @@
   </si>
   <si>
     <t>陈泽鑫</t>
+  </si>
+  <si>
+    <t>陈安怡
+test</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -222,16 +232,16 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -241,7 +251,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -259,6 +269,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -542,18 +555,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B10" sqref="B9:B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="2" max="2" width="10.85546875" customWidth="1"/>
+    <col min="2" max="2" width="10.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B1" s="2">
         <v>34</v>
@@ -563,14 +576,14 @@
       </c>
       <c r="D1" s="3">
         <f t="shared" ref="D1:D42" ca="1" si="0">RANDBETWEEN(0,100)</f>
-        <v>41</v>
+        <v>61</v>
       </c>
       <c r="E1">
         <f>B1/C1</f>
         <v>2.4285714285714284</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -582,14 +595,14 @@
       </c>
       <c r="D2" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>74</v>
+        <v>47</v>
       </c>
       <c r="E2">
         <f t="shared" ref="E2:E42" si="1">B2/C2</f>
         <v>1.1111111111111112E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -601,14 +614,14 @@
       </c>
       <c r="D3" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>72</v>
+        <v>2</v>
       </c>
       <c r="E3">
         <f t="shared" si="1"/>
         <v>0.26415094339622641</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
@@ -620,16 +633,16 @@
       </c>
       <c r="D4" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>40</v>
+        <v>24</v>
       </c>
       <c r="E4">
         <f t="shared" si="1"/>
         <v>0.5</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>8</v>
+    <row r="5" spans="1:5" ht="28" x14ac:dyDescent="0.15">
+      <c r="A5" s="6" t="s">
+        <v>41</v>
       </c>
       <c r="B5" s="2">
         <v>18</v>
@@ -639,16 +652,16 @@
       </c>
       <c r="D5" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="E5">
         <f t="shared" si="1"/>
         <v>3.6</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A6" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B6" s="2">
         <v>83.12133</v>
@@ -658,16 +671,16 @@
       </c>
       <c r="D6" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>59</v>
+        <v>11</v>
       </c>
       <c r="E6">
         <f t="shared" si="1"/>
         <v>20.7803325</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A7" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B7" s="2">
         <v>44</v>
@@ -677,14 +690,14 @@
       </c>
       <c r="D7" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>72</v>
       </c>
       <c r="E7">
         <f t="shared" si="1"/>
         <v>0.54320987654320985</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A8" s="2" t="s">
         <v>4</v>
       </c>
@@ -696,16 +709,16 @@
       </c>
       <c r="D8" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="E8">
         <f t="shared" si="1"/>
         <v>0.10112359550561797</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A9" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B9" s="2">
         <v>45</v>
@@ -722,9 +735,9 @@
         <v>3.2142857142857144</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A10" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B10" s="2">
         <v>81</v>
@@ -734,16 +747,16 @@
       </c>
       <c r="D10" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="E10">
         <f t="shared" si="1"/>
         <v>1.051948051948052</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A11" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B11" s="2">
         <v>28</v>
@@ -753,14 +766,14 @@
       </c>
       <c r="D11" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>78</v>
+        <v>61</v>
       </c>
       <c r="E11">
         <f t="shared" si="1"/>
         <v>0.84848484848484851</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A12" s="2" t="s">
         <v>5</v>
       </c>
@@ -772,16 +785,16 @@
       </c>
       <c r="D12" s="3">
         <f ca="1">RANDBETWEEN(0,100)</f>
-        <v>11</v>
+        <v>89</v>
       </c>
       <c r="E12">
         <f t="shared" si="1"/>
         <v>0.8</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A13" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B13" s="2">
         <v>58</v>
@@ -791,16 +804,16 @@
       </c>
       <c r="D13" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>52</v>
+        <v>79</v>
       </c>
       <c r="E13">
         <f t="shared" si="1"/>
         <v>1.9333333333333333</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A14" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B14" s="4">
         <v>84</v>
@@ -810,16 +823,16 @@
       </c>
       <c r="D14" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>48</v>
+        <v>79</v>
       </c>
       <c r="E14">
         <f t="shared" si="1"/>
         <v>1.1351351351351351</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A15" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15" s="4">
         <v>30</v>
@@ -829,16 +842,16 @@
       </c>
       <c r="D15" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>30</v>
+        <v>69</v>
       </c>
       <c r="E15">
         <f t="shared" si="1"/>
         <v>0.78947368421052633</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A16" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B16" s="4">
         <v>38</v>
@@ -848,14 +861,14 @@
       </c>
       <c r="D16" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>97</v>
+        <v>49</v>
       </c>
       <c r="E16">
         <f t="shared" si="1"/>
         <v>1.6521739130434783</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A17" s="4" t="s">
         <v>2</v>
       </c>
@@ -867,16 +880,16 @@
       </c>
       <c r="D17" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>26</v>
+        <v>49</v>
       </c>
       <c r="E17">
         <f t="shared" si="1"/>
         <v>6.4516129032258063E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A18" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B18" s="4">
         <v>64</v>
@@ -886,16 +899,16 @@
       </c>
       <c r="D18" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v>72</v>
       </c>
       <c r="E18">
         <f t="shared" si="1"/>
         <v>1.3333333333333333</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A19" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B19" s="4">
         <v>24</v>
@@ -905,16 +918,16 @@
       </c>
       <c r="D19" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="E19">
         <f t="shared" si="1"/>
         <v>0.3380281690140845</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A20" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B20" s="4">
         <v>52</v>
@@ -924,14 +937,14 @@
       </c>
       <c r="D20" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>86</v>
+        <v>55</v>
       </c>
       <c r="E20">
         <f t="shared" si="1"/>
         <v>0.55913978494623651</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A21" s="4" t="s">
         <v>3</v>
       </c>
@@ -943,16 +956,16 @@
       </c>
       <c r="D21" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="E21">
         <f t="shared" si="1"/>
         <v>0.4375</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A22" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B22" s="4">
         <v>73</v>
@@ -962,16 +975,16 @@
       </c>
       <c r="D22" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v>64</v>
       </c>
       <c r="E22">
         <f t="shared" si="1"/>
         <v>3.3181818181818183</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A23" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B23" s="4">
         <v>71</v>
@@ -981,16 +994,16 @@
       </c>
       <c r="D23" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>52</v>
+        <v>80</v>
       </c>
       <c r="E23">
         <f t="shared" si="1"/>
         <v>1.6136363636363635</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A24" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B24" s="4">
         <v>57</v>
@@ -1000,14 +1013,14 @@
       </c>
       <c r="D24" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>99</v>
+        <v>9</v>
       </c>
       <c r="E24">
         <f t="shared" si="1"/>
         <v>1.3902439024390243</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A25" s="4" t="s">
         <v>1</v>
       </c>
@@ -1019,16 +1032,16 @@
       </c>
       <c r="D25" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>100</v>
+        <v>42</v>
       </c>
       <c r="E25">
         <f t="shared" si="1"/>
         <v>8.1081081081081086E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A26" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B26" s="4">
         <v>65</v>
@@ -1038,16 +1051,16 @@
       </c>
       <c r="D26" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="E26">
         <f t="shared" si="1"/>
         <v>0.98484848484848486</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A27" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B27" s="4">
         <v>55</v>
@@ -1057,16 +1070,16 @@
       </c>
       <c r="D27" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>60</v>
       </c>
       <c r="E27">
         <f t="shared" si="1"/>
         <v>0.88709677419354838</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A28" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B28" s="4">
         <v>80</v>
@@ -1076,16 +1089,16 @@
       </c>
       <c r="D28" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="E28">
         <f t="shared" si="1"/>
         <v>5.7142857142857144</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A29" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B29" s="5">
         <v>54</v>
@@ -1095,16 +1108,16 @@
       </c>
       <c r="D29" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>38</v>
+        <v>5</v>
       </c>
       <c r="E29">
         <f t="shared" si="1"/>
         <v>54</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A30" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B30" s="5">
         <v>40</v>
@@ -1114,16 +1127,16 @@
       </c>
       <c r="D30" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="E30">
         <f>B30/C30</f>
         <v>0.48780487804878048</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A31" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B31" s="5">
         <v>21</v>
@@ -1133,16 +1146,16 @@
       </c>
       <c r="D31" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="E31">
         <f t="shared" si="1"/>
         <v>1.1666666666666667</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A32" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B32" s="5">
         <v>37</v>
@@ -1152,16 +1165,16 @@
       </c>
       <c r="D32" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>36</v>
       </c>
       <c r="E32">
         <f t="shared" si="1"/>
         <v>2.8461538461538463</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A33" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B33" s="5">
         <v>70</v>
@@ -1171,16 +1184,16 @@
       </c>
       <c r="D33" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>99</v>
+        <v>49</v>
       </c>
       <c r="E33">
         <f t="shared" si="1"/>
         <v>1.5217391304347827</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A34" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B34" s="5">
         <v>43</v>
@@ -1190,16 +1203,16 @@
       </c>
       <c r="D34" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>60</v>
+        <v>69</v>
       </c>
       <c r="E34">
         <f t="shared" si="1"/>
         <v>1.5357142857142858</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A35" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B35" s="5">
         <v>76</v>
@@ -1209,16 +1222,16 @@
       </c>
       <c r="D35" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="E35">
         <f t="shared" si="1"/>
         <v>5.4285714285714288</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A36" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B36" s="5">
         <v>25</v>
@@ -1228,16 +1241,16 @@
       </c>
       <c r="D36" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>67</v>
+        <v>41</v>
       </c>
       <c r="E36">
         <f t="shared" si="1"/>
         <v>6.25</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A37" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B37" s="5">
         <v>31</v>
@@ -1247,16 +1260,16 @@
       </c>
       <c r="D37" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>72</v>
+        <v>27</v>
       </c>
       <c r="E37">
         <f t="shared" si="1"/>
         <v>2.5833333333333335</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A38" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B38" s="5">
         <v>67</v>
@@ -1266,16 +1279,16 @@
       </c>
       <c r="D38" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>24</v>
+        <v>77</v>
       </c>
       <c r="E38">
         <f t="shared" si="1"/>
         <v>2.3103448275862069</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A39" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B39" s="5">
         <v>48</v>
@@ -1285,16 +1298,16 @@
       </c>
       <c r="D39" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>92</v>
+        <v>31</v>
       </c>
       <c r="E39">
         <f t="shared" si="1"/>
         <v>0.48</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A40" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B40" s="5">
         <v>56</v>
@@ -1304,16 +1317,16 @@
       </c>
       <c r="D40" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>10</v>
+        <v>42</v>
       </c>
       <c r="E40">
         <f t="shared" si="1"/>
         <v>0.7</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A41" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B41" s="5">
         <v>26</v>
@@ -1323,16 +1336,16 @@
       </c>
       <c r="D41" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>99</v>
+        <v>78</v>
       </c>
       <c r="E41">
         <f t="shared" si="1"/>
         <v>0.60465116279069764</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A42" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B42" s="5">
         <v>32</v>
@@ -1342,7 +1355,7 @@
       </c>
       <c r="D42" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>29</v>
+        <v>93</v>
       </c>
       <c r="E42">
         <f t="shared" si="1"/>

</xml_diff>